<commit_message>
add cpu % metric to data-set
</commit_message>
<xml_diff>
--- a/data-set/i-0d0742ad676ee9a46.xlsx
+++ b/data-set/i-0d0742ad676ee9a46.xlsx
@@ -1,46 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Hour</t>
-  </si>
-  <si>
-    <t>CPU Utilization</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -59,13 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -353,22 +407,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hour</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>CPU Utilization</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2021-03-30</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>21:28:27</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.508474576271109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add aws sdk integration
</commit_message>
<xml_diff>
--- a/data-set/i-0d0742ad676ee9a46.xlsx
+++ b/data-set/i-0d0742ad676ee9a46.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,6 +572,66 @@
         <v>0.500000000000303</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>01:38:03</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.4350838195794973</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>01:39:21</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4339909234046336</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>01:40:05</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.4339909234046336</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>01:41:07</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.4328980272297699</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add scale up and down
</commit_message>
<xml_diff>
--- a/data-set/i-0d0742ad676ee9a46.xlsx
+++ b/data-set/i-0d0742ad676ee9a46.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,524 @@
         <v>26.4</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>19:03:47</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.46502732240440076</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3958.8</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>7470.0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>36.0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>19:04:44</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.43282393257377</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3657.0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>5547.4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>36.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>19:05:03</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.43118458831162554</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2964.4</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>4786.6</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>36.0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>19:05:46</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.43118458831162554</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2964.4</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4786.6</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>36.0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>19:06:45</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.4328239325739216</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2942.0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4765.0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>36.0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>19:07:45</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.43282393257377</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3073.2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>4951.4</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>36.0</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>19:08:45</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.467852181161463</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3102.4</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4972.2</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>19:09:46</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.4667222376586392</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3120.4</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>4987.4</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>19:10:45</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0.46836158192093513</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3277.4</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5063.8</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19:11:20</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.432877710953074</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3349.8</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>5105.4</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>19:11:45</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.432877710953074</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>3349.8</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>5105.4</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>19:12:45</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0.43632598681529683</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3194.4</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>5100.0</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>27.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>19:13:44</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.43299172729861324</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3281.6</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>5159.2</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>39.4</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>28.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2021-04-02</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19:13:45</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.43299172729861324</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3281.6</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>5159.2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>39.4</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>28.0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>